<commit_message>
update .... matrix from arif
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_37.xlsx
+++ b/test_case_report/sprint_37.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD08621A-15A1-4B34-BE97-1A45B900A14B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF94CAF4-9D67-4B05-8CF2-708D773C48A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>Total  testcase Written</t>
   </si>
@@ -36,10 +36,10 @@
     <t>Total Review</t>
   </si>
   <si>
-    <t>Spint( 36) - Day 1 - Test Case Summary</t>
+    <t>Spint( 3) - Day 2 - Test Case Summary</t>
   </si>
   <si>
-    <t>Spint( 36) - Day 2 - Test Case Summary</t>
+    <t>Spint( 3) - Day 1 - Test Case Summary</t>
   </si>
 </sst>
 </file>
@@ -516,25 +516,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
@@ -550,7 +550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -558,13 +558,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="2:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
         <v>0</v>
       </c>
@@ -572,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -580,7 +580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="18" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>2</v>
       </c>
@@ -588,10 +588,41 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="B16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>173</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sprint updated day 5
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_37.xlsx
+++ b/test_case_report/sprint_37.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases_bk\test_case_report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85365EED-898B-4F5C-A7D7-E053C572EC5A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA517AF-B398-4B44-BDBE-F79DE93692BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="B2:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>10</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">

</xml_diff>